<commit_message>
SpeedRunMode and Free camera
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26719"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\AGA206\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlooyen1\workspace\AGA206\Roll-A-Ball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F0CCB8C-1A20-4268-9262-E45BB8B7DC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -140,12 +139,15 @@
   <si>
     <t>Come up with your own</t>
   </si>
+  <si>
+    <t>NPC with dialogue</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -432,7 +434,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,7 +478,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -504,11 +506,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2473,14 +2475,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="6.125" style="2" bestFit="1" customWidth="1"/>
@@ -2497,15 +2499,15 @@
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="15.75">
+    <row r="2" spans="2:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C2" s="23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
@@ -2516,7 +2518,7 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
@@ -2527,20 +2529,20 @@
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="8">
         <f>COUNTIFS(J12:J15,TRUE)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C8" s="7" t="s">
         <v>4</v>
       </c>
@@ -2549,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C9" s="7" t="s">
         <v>5</v>
       </c>
@@ -2558,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2579,7 +2581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <v>1</v>
       </c>
@@ -2592,14 +2594,14 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6" t="str">
         <f>IF(J12,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G12" s="17"/>
       <c r="J12" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <v>2</v>
       </c>
@@ -2612,14 +2614,14 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6" t="str">
         <f>IF(J13,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G13" s="17"/>
       <c r="J13" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1">
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <v>3</v>
       </c>
@@ -2632,14 +2634,14 @@
       <c r="E14" s="7"/>
       <c r="F14" s="6" t="str">
         <f>IF(J14,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G14" s="17"/>
       <c r="J14" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <v>4</v>
       </c>
@@ -2652,17 +2654,17 @@
       <c r="E15" s="7"/>
       <c r="F15" s="6" t="str">
         <f>IF(J15,"Done","To Be Done")</f>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G15" s="17"/>
       <c r="J15" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
     </row>
-    <row r="17" spans="2:11" ht="15" customHeight="1">
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
         <v>6</v>
       </c>
@@ -2680,7 +2682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>5</v>
       </c>
@@ -2704,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="6">
         <v>6</v>
       </c>
@@ -2728,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <v>7</v>
       </c>
@@ -2752,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="6">
         <v>8</v>
       </c>
@@ -2776,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <v>9</v>
       </c>
@@ -2800,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="6">
         <v>10</v>
       </c>
@@ -2824,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="6">
         <v>11</v>
       </c>
@@ -2848,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="6">
         <v>12</v>
       </c>
@@ -2872,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="6">
         <v>13</v>
       </c>
@@ -2896,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="6">
         <v>14</v>
       </c>
@@ -2920,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="6">
         <v>15</v>
       </c>
@@ -2944,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="6">
         <v>16</v>
       </c>
@@ -2968,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="6">
         <v>17</v>
       </c>
@@ -2992,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="6">
         <v>18</v>
       </c>
@@ -3016,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="6">
         <v>19</v>
       </c>
@@ -3040,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="6">
         <v>20</v>
       </c>
@@ -3064,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="6">
         <v>21</v>
       </c>
@@ -3088,12 +3090,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="6">
         <v>22</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" s="19">
         <v>2</v>
@@ -3112,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="6">
         <v>23</v>
       </c>
@@ -3136,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="6">
         <v>24</v>
       </c>
@@ -3160,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="6">
         <v>25</v>
       </c>
@@ -3184,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
         <v>0</v>
@@ -3795,6 +3797,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5A66FD54D20CA4E9AC02DD318E94D49" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53bde79962055b8cecc8a50be1004eac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de" xmlns:ns3="c2062536-d537-4933-9a68-111b11088bac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d9b45dcf71f2936b8953ced3331ea195" ns2:_="" ns3:_="">
     <xsd:import namespace="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
@@ -4037,23 +4048,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c2062536-d537-4933-9a68-111b11088bac"/>
+    <ds:schemaRef ds:uri="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E3157D-E74E-4DE5-B0FD-8DBD0694FA2F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7E3157D-E74E-4DE5-B0FD-8DBD0694FA2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
+    <ds:schemaRef ds:uri="c2062536-d537-4933-9a68-111b11088bac"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed NPCS added right/wrong
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Charlie Looyen</t>
+  </si>
+  <si>
+    <t>lock and key</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2484,8 +2487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2556,7 +2559,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2565,7 +2568,7 @@
       </c>
       <c r="D9" s="8">
         <f>K39 + E9</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2754,15 +2757,15 @@
       <c r="E20" s="7"/>
       <c r="F20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
+        <v>Done</v>
       </c>
       <c r="G20" s="17"/>
       <c r="J20" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
@@ -3154,10 +3157,10 @@
         <v>24</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D37" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="6" t="str">
@@ -3200,7 +3203,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3797,15 +3800,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c2062536-d537-4933-9a68-111b11088bac" xsi:nil="true"/>
@@ -3814,6 +3808,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4060,20 +4063,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F4C952-2792-4F13-AAE1-711BCAAD3EBE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="c2062536-d537-4933-9a68-111b11088bac"/>
     <ds:schemaRef ds:uri="aabe51d3-f54d-4fdd-9fcd-70ffe0d760de"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14E3574E-6B93-421F-8C9B-EF2BAE2A1531}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
finalised game, ready for build
</commit_message>
<xml_diff>
--- a/AGA206 Assessment 2 Checklist.xlsx
+++ b/AGA206 Assessment 2 Checklist.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -151,12 +151,15 @@
   <si>
     <t>Points system</t>
   </si>
+  <si>
+    <t>https://github.com/Etheratic/Roll-A-Ball</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -185,6 +188,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -296,10 +306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -361,7 +372,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -373,8 +384,13 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -2487,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2520,7 +2536,7 @@
       <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="27" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="25"/>
@@ -2533,7 +2549,9 @@
       <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
       <c r="G5" s="26"/>
@@ -3236,16 +3254,19 @@
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId4" name="Check Box 11">
+            <control shapeId="1035" r:id="rId5" name="Check Box 11">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3267,7 +3288,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId5" name="Check Box 12">
+            <control shapeId="1036" r:id="rId6" name="Check Box 12">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3289,7 +3310,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId6" name="Check Box 13">
+            <control shapeId="1037" r:id="rId7" name="Check Box 13">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3311,7 +3332,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId7" name="Check Box 14">
+            <control shapeId="1038" r:id="rId8" name="Check Box 14">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3333,7 +3354,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1054" r:id="rId8" name="Check Box 30">
+            <control shapeId="1054" r:id="rId9" name="Check Box 30">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3355,7 +3376,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1055" r:id="rId9" name="Check Box 31">
+            <control shapeId="1055" r:id="rId10" name="Check Box 31">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3377,7 +3398,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId10" name="Check Box 32">
+            <control shapeId="1056" r:id="rId11" name="Check Box 32">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3399,7 +3420,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1057" r:id="rId11" name="Check Box 33">
+            <control shapeId="1057" r:id="rId12" name="Check Box 33">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3421,7 +3442,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1059" r:id="rId12" name="Check Box 35">
+            <control shapeId="1059" r:id="rId13" name="Check Box 35">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3443,7 +3464,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1060" r:id="rId13" name="Check Box 36">
+            <control shapeId="1060" r:id="rId14" name="Check Box 36">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3465,7 +3486,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1062" r:id="rId14" name="Check Box 38">
+            <control shapeId="1062" r:id="rId15" name="Check Box 38">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3487,7 +3508,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1063" r:id="rId15" name="Check Box 39">
+            <control shapeId="1063" r:id="rId16" name="Check Box 39">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3509,7 +3530,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId16" name="Check Box 41">
+            <control shapeId="1065" r:id="rId17" name="Check Box 41">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3531,7 +3552,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1066" r:id="rId17" name="Check Box 42">
+            <control shapeId="1066" r:id="rId18" name="Check Box 42">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3553,7 +3574,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1067" r:id="rId18" name="Check Box 43">
+            <control shapeId="1067" r:id="rId19" name="Check Box 43">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3575,7 +3596,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1068" r:id="rId19" name="Check Box 44">
+            <control shapeId="1068" r:id="rId20" name="Check Box 44">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3597,7 +3618,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1070" r:id="rId20" name="Check Box 46">
+            <control shapeId="1070" r:id="rId21" name="Check Box 46">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3619,7 +3640,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1071" r:id="rId21" name="Check Box 47">
+            <control shapeId="1071" r:id="rId22" name="Check Box 47">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3641,7 +3662,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1072" r:id="rId22" name="Check Box 48">
+            <control shapeId="1072" r:id="rId23" name="Check Box 48">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3663,7 +3684,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1073" r:id="rId23" name="Check Box 49">
+            <control shapeId="1073" r:id="rId24" name="Check Box 49">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3685,7 +3706,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1075" r:id="rId24" name="Check Box 51">
+            <control shapeId="1075" r:id="rId25" name="Check Box 51">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3707,7 +3728,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1076" r:id="rId25" name="Check Box 52">
+            <control shapeId="1076" r:id="rId26" name="Check Box 52">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3729,7 +3750,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1077" r:id="rId26" name="Check Box 53">
+            <control shapeId="1077" r:id="rId27" name="Check Box 53">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3751,7 +3772,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1078" r:id="rId27" name="Check Box 54">
+            <control shapeId="1078" r:id="rId28" name="Check Box 54">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3773,7 +3794,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1079" r:id="rId28" name="Check Box 55">
+            <control shapeId="1079" r:id="rId29" name="Check Box 55">
               <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>